<commit_message>
update hard ware, firmware, datasheet
</commit_message>
<xml_diff>
--- a/PCB/Component List/component.xlsx
+++ b/PCB/Component List/component.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LE TUAN THANH\Downloads\tai lieu\ĐHBK\Năm 4\233\Project\PCB\Component List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B63A7-9ED0-4229-94F4-871FBEFD7C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89D9AC3-3138-4D97-965D-0237A0722167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60C50E94-620A-441F-8BC0-7ADFEAA2EE58}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>STT</t>
   </si>
@@ -53,8 +53,20 @@
     <t>MAX30102 ( đọc nhịp tim)</t>
   </si>
   <si>
+    <t>Màn hình Oled</t>
+  </si>
+  <si>
+    <t>Kiểu đóng gói</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQFP48 </t>
+  </si>
+  <si>
+    <t>Điện trở 100kΩ</t>
+  </si>
+  <si>
     <r>
-      <t>Điện trở 1k</t>
+      <t>Điện trở 10k</t>
     </r>
     <r>
       <rPr>
@@ -66,12 +78,48 @@
       <t>Ω</t>
     </r>
   </si>
+  <si>
+    <t>Điện trở 20Ω</t>
+  </si>
+  <si>
+    <t>Điện trở 4.7kΩ</t>
+  </si>
+  <si>
+    <t>Điện trở 1MΩ</t>
+  </si>
+  <si>
+    <t>Điện trở 510Ω</t>
+  </si>
+  <si>
+    <t>SMD 0603</t>
+  </si>
+  <si>
+    <t>RT9193-33</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>Tụ gốm 10uF</t>
+  </si>
+  <si>
+    <t>Tụ gốm 22nF</t>
+  </si>
+  <si>
+    <t>Tụ gốm 1uF</t>
+  </si>
+  <si>
+    <t>Tụ gốm 100nF</t>
+  </si>
+  <si>
+    <t>Tụ gốm 20pF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +142,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -115,12 +170,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -457,80 +518,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1894E8F-5C54-4F91-AB0A-AC261E82E06C}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="36.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="24.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>